<commit_message>
Fixed BoM and PnP files for CH340G and FT232RL boards.
</commit_message>
<xml_diff>
--- a/cam/USB2Serial_CH340G_v1.2_2021-04-08-BoM.xlsx
+++ b/cam/USB2Serial_CH340G_v1.2_2021-04-08-BoM.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\USB2Serial\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7161E486-C96D-4E7C-9FF0-C79360A55E89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0390E97E-FEED-4CDF-A3F7-5DC5135FCE59}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19450" yWindow="100" windowWidth="20910" windowHeight="20770" activeTab="1" xr2:uid="{58888B4C-DAFF-4F57-B125-37D2187AF46A}"/>
+    <workbookView xWindow="24330" yWindow="840" windowWidth="16430" windowHeight="19950" xr2:uid="{58888B4C-DAFF-4F57-B125-37D2187AF46A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Sheet2!$A$1:$D$14</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet1!$A$1:$D$14</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -622,18 +621,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9484F2A1-56B1-4E00-A7A0-B1F116E245AE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5B149E-4BCC-4C3B-AC2A-D853BC085718}">
   <dimension ref="A1:E14"/>
   <sheetViews>

</xml_diff>